<commit_message>
Kigali Rainfall of 2024 Adjustment and code upadte
</commit_message>
<xml_diff>
--- a/Data/UNILAK/Rainfall and Temprature.xlsx
+++ b/Data/UNILAK/Rainfall and Temprature.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chukw\Documents\KingVik Planet\Geomatics\KingVik Planet\Fabrice MUVUNYI  EIS UNILAK\Maps and Analysis\Temprature and Rainfall\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chukw\PycharmProjects\Kingsley Chika CHUKWU _AcadProject\Data\UNILAK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732245D5-E5EF-47E5-853E-EC5CFB4EF065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5608AF8A-98B5-45B1-B5CF-643173EAA88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{2E3629EA-C96F-4C30-910D-7543223C5EFB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2E3629EA-C96F-4C30-910D-7543223C5EFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E09538-DCF6-4C93-88E2-C6585D37003F}">
   <dimension ref="A1:L1097"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="B1077" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N1102" sqref="N1102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26534,7 +26534,7 @@
         <v>1</v>
       </c>
       <c r="I732" s="1">
-        <v>4.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="J732" s="1">
         <v>26.1</v>
@@ -26569,7 +26569,7 @@
         <v>2</v>
       </c>
       <c r="I733" s="1">
-        <v>1.4</v>
+        <v>0.19</v>
       </c>
       <c r="J733" s="1">
         <v>27.6</v>
@@ -26604,7 +26604,7 @@
         <v>3</v>
       </c>
       <c r="I734" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J734" s="1">
         <v>28.8</v>
@@ -26744,7 +26744,7 @@
         <v>7</v>
       </c>
       <c r="I738" s="1">
-        <v>21.4</v>
+        <v>0</v>
       </c>
       <c r="J738" s="1">
         <v>28.9</v>
@@ -26849,7 +26849,7 @@
         <v>10</v>
       </c>
       <c r="I741" s="1">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="J741" s="1">
         <v>29.6</v>
@@ -26884,7 +26884,7 @@
         <v>11</v>
       </c>
       <c r="I742" s="1">
-        <v>37.6</v>
+        <v>0.22</v>
       </c>
       <c r="J742" s="1">
         <v>29.1</v>
@@ -26954,7 +26954,7 @@
         <v>13</v>
       </c>
       <c r="I744" s="1">
-        <v>16.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="J744" s="1">
         <v>30.4</v>
@@ -26989,7 +26989,7 @@
         <v>14</v>
       </c>
       <c r="I745" s="1">
-        <v>3.4</v>
+        <v>0.79</v>
       </c>
       <c r="J745" s="1">
         <v>31</v>
@@ -27024,7 +27024,7 @@
         <v>15</v>
       </c>
       <c r="I746" s="1">
-        <v>34</v>
+        <v>1.46</v>
       </c>
       <c r="J746" s="1">
         <v>29.8</v>
@@ -27094,7 +27094,7 @@
         <v>17</v>
       </c>
       <c r="I748" s="1">
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="J748" s="1">
         <v>29</v>
@@ -27129,7 +27129,7 @@
         <v>18</v>
       </c>
       <c r="I749" s="1">
-        <v>7.8</v>
+        <v>0.17</v>
       </c>
       <c r="J749" s="1">
         <v>31</v>
@@ -27164,7 +27164,7 @@
         <v>19</v>
       </c>
       <c r="I750" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J750" s="1">
         <v>31.8</v>
@@ -27199,7 +27199,7 @@
         <v>20</v>
       </c>
       <c r="I751" s="1">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="J751" s="1">
         <v>27.2</v>
@@ -27269,7 +27269,7 @@
         <v>22</v>
       </c>
       <c r="I753" s="1">
-        <v>7.8</v>
+        <v>0</v>
       </c>
       <c r="J753" s="1">
         <v>27.5</v>
@@ -27339,7 +27339,7 @@
         <v>24</v>
       </c>
       <c r="I755" s="1">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="J755" s="1">
         <v>28.3</v>
@@ -27409,7 +27409,7 @@
         <v>26</v>
       </c>
       <c r="I757" s="1">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="J757" s="1">
         <v>31.6</v>
@@ -27549,7 +27549,7 @@
         <v>30</v>
       </c>
       <c r="I761" s="1">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="J761" s="1">
         <v>24</v>
@@ -27617,7 +27617,7 @@
         <v>1</v>
       </c>
       <c r="I763" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="J763" s="1">
         <v>22.9</v>
@@ -27652,7 +27652,7 @@
         <v>2</v>
       </c>
       <c r="I764" s="1">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="J764" s="1">
         <v>26.7</v>
@@ -27687,7 +27687,7 @@
         <v>3</v>
       </c>
       <c r="I765" s="1">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="J765" s="1">
         <v>25</v>
@@ -27757,7 +27757,7 @@
         <v>5</v>
       </c>
       <c r="I767" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J767" s="1">
         <v>24.5</v>
@@ -27792,7 +27792,7 @@
         <v>6</v>
       </c>
       <c r="I768" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J768" s="1">
         <v>27.1</v>
@@ -27897,7 +27897,7 @@
         <v>9</v>
       </c>
       <c r="I771" s="1">
-        <v>2.4</v>
+        <v>0.2</v>
       </c>
       <c r="J771" s="1">
         <v>29</v>
@@ -27932,7 +27932,7 @@
         <v>10</v>
       </c>
       <c r="I772" s="1">
-        <v>6.6</v>
+        <v>0</v>
       </c>
       <c r="J772" s="1">
         <v>23.7</v>
@@ -28072,7 +28072,7 @@
         <v>14</v>
       </c>
       <c r="I776" s="1">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J776" s="1">
         <v>30.5</v>
@@ -28107,7 +28107,7 @@
         <v>15</v>
       </c>
       <c r="I777" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J777" s="1">
         <v>24.2</v>
@@ -28142,7 +28142,7 @@
         <v>16</v>
       </c>
       <c r="I778" s="1">
-        <v>7.2</v>
+        <v>0</v>
       </c>
       <c r="J778" s="1">
         <v>26.7</v>
@@ -28247,7 +28247,7 @@
         <v>19</v>
       </c>
       <c r="I781" s="1">
-        <v>17.3</v>
+        <v>0</v>
       </c>
       <c r="J781" s="1">
         <v>28.1</v>
@@ -28282,7 +28282,7 @@
         <v>20</v>
       </c>
       <c r="I782" s="1">
-        <v>18.399999999999999</v>
+        <v>0</v>
       </c>
       <c r="J782" s="1">
         <v>28.4</v>
@@ -28317,7 +28317,7 @@
         <v>21</v>
       </c>
       <c r="I783" s="1">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="J783" s="1">
         <v>28.8</v>
@@ -28352,7 +28352,7 @@
         <v>22</v>
       </c>
       <c r="I784" s="1">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="J784" s="1">
         <v>27.6</v>
@@ -28422,7 +28422,7 @@
         <v>24</v>
       </c>
       <c r="I786" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="J786" s="1">
         <v>28.7</v>
@@ -28457,7 +28457,7 @@
         <v>25</v>
       </c>
       <c r="I787" s="1">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="J787" s="1">
         <v>29.3</v>
@@ -28492,7 +28492,7 @@
         <v>26</v>
       </c>
       <c r="I788" s="1">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="J788" s="1">
         <v>21.9</v>
@@ -28527,7 +28527,7 @@
         <v>27</v>
       </c>
       <c r="I789" s="1">
-        <v>0</v>
+        <v>11.4</v>
       </c>
       <c r="J789" s="1">
         <v>22.8</v>
@@ -28562,7 +28562,7 @@
         <v>28</v>
       </c>
       <c r="I790" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J790" s="1">
         <v>25.5</v>
@@ -28597,7 +28597,7 @@
         <v>29</v>
       </c>
       <c r="I791" s="1">
-        <v>24.4</v>
+        <v>0</v>
       </c>
       <c r="J791" s="1">
         <v>30.3</v>
@@ -28667,7 +28667,7 @@
         <v>2</v>
       </c>
       <c r="I793" s="1">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="J793" s="1">
         <v>26.2</v>
@@ -28702,7 +28702,7 @@
         <v>3</v>
       </c>
       <c r="I794" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J794" s="1">
         <v>28.6</v>
@@ -28772,7 +28772,7 @@
         <v>5</v>
       </c>
       <c r="I796" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="J796" s="1">
         <v>25.1</v>
@@ -28807,7 +28807,7 @@
         <v>6</v>
       </c>
       <c r="I797" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J797" s="1">
         <v>23.6</v>
@@ -28842,7 +28842,7 @@
         <v>7</v>
       </c>
       <c r="I798" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J798" s="1">
         <v>27.9</v>
@@ -28877,7 +28877,7 @@
         <v>8</v>
       </c>
       <c r="I799" s="1">
-        <v>7.6</v>
+        <v>0</v>
       </c>
       <c r="J799" s="1">
         <v>29.1</v>
@@ -28912,7 +28912,7 @@
         <v>9</v>
       </c>
       <c r="I800" s="1">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="J800" s="1">
         <v>23.8</v>
@@ -28982,7 +28982,7 @@
         <v>11</v>
       </c>
       <c r="I802" s="1">
-        <v>0</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="J802" s="1">
         <v>28</v>
@@ -29017,7 +29017,7 @@
         <v>12</v>
       </c>
       <c r="I803" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J803" s="1">
         <v>28.9</v>
@@ -29052,7 +29052,7 @@
         <v>13</v>
       </c>
       <c r="I804" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J804" s="1">
         <v>30.3</v>
@@ -29087,7 +29087,7 @@
         <v>14</v>
       </c>
       <c r="I805" s="1">
-        <v>0.2</v>
+        <v>26.4</v>
       </c>
       <c r="J805" s="1">
         <v>28.1</v>
@@ -29157,7 +29157,7 @@
         <v>16</v>
       </c>
       <c r="I807" s="1">
-        <v>0</v>
+        <v>29.1</v>
       </c>
       <c r="J807" s="1">
         <v>29.2</v>
@@ -29227,7 +29227,7 @@
         <v>18</v>
       </c>
       <c r="I809" s="1">
-        <v>0</v>
+        <v>9.9</v>
       </c>
       <c r="J809" s="1">
         <v>30.2</v>
@@ -29262,7 +29262,7 @@
         <v>19</v>
       </c>
       <c r="I810" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J810" s="1">
         <v>29.9</v>
@@ -29296,7 +29296,9 @@
       <c r="H811" s="1">
         <v>20</v>
       </c>
-      <c r="I811" s="1"/>
+      <c r="I811" s="1">
+        <v>12.9</v>
+      </c>
       <c r="J811" s="1">
         <v>28.3</v>
       </c>
@@ -29329,7 +29331,9 @@
       <c r="H812" s="1">
         <v>21</v>
       </c>
-      <c r="I812" s="1"/>
+      <c r="I812" s="1">
+        <v>0.3</v>
+      </c>
       <c r="J812" s="1">
         <v>29.2</v>
       </c>
@@ -29362,7 +29366,9 @@
       <c r="H813" s="1">
         <v>22</v>
       </c>
-      <c r="I813" s="1"/>
+      <c r="I813" s="1">
+        <v>24.4</v>
+      </c>
       <c r="J813" s="1">
         <v>27</v>
       </c>
@@ -29395,7 +29401,9 @@
       <c r="H814" s="1">
         <v>23</v>
       </c>
-      <c r="I814" s="1"/>
+      <c r="I814" s="1">
+        <v>2</v>
+      </c>
       <c r="J814" s="1">
         <v>26.2</v>
       </c>
@@ -29428,7 +29436,9 @@
       <c r="H815" s="1">
         <v>24</v>
       </c>
-      <c r="I815" s="1"/>
+      <c r="I815" s="1">
+        <v>0.8</v>
+      </c>
       <c r="J815" s="1">
         <v>26.9</v>
       </c>
@@ -29461,7 +29471,9 @@
       <c r="H816" s="1">
         <v>25</v>
       </c>
-      <c r="I816" s="1"/>
+      <c r="I816" s="1">
+        <v>0</v>
+      </c>
       <c r="J816" s="1">
         <v>28.8</v>
       </c>
@@ -29494,7 +29506,9 @@
       <c r="H817" s="1">
         <v>26</v>
       </c>
-      <c r="I817" s="1"/>
+      <c r="I817" s="1">
+        <v>8.9</v>
+      </c>
       <c r="J817" s="1">
         <v>27.8</v>
       </c>
@@ -29527,7 +29541,9 @@
       <c r="H818" s="1">
         <v>27</v>
       </c>
-      <c r="I818" s="1"/>
+      <c r="I818" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J818" s="1">
         <v>24.6</v>
       </c>
@@ -29560,7 +29576,9 @@
       <c r="H819" s="1">
         <v>28</v>
       </c>
-      <c r="I819" s="1"/>
+      <c r="I819" s="1">
+        <v>0</v>
+      </c>
       <c r="J819" s="1">
         <v>27.8</v>
       </c>
@@ -29593,7 +29611,9 @@
       <c r="H820" s="1">
         <v>29</v>
       </c>
-      <c r="I820" s="1"/>
+      <c r="I820" s="1">
+        <v>0</v>
+      </c>
       <c r="J820" s="1">
         <v>25</v>
       </c>
@@ -29626,7 +29646,9 @@
       <c r="H821" s="1">
         <v>30</v>
       </c>
-      <c r="I821" s="1"/>
+      <c r="I821" s="1">
+        <v>4.3</v>
+      </c>
       <c r="J821" s="1">
         <v>28.8</v>
       </c>
@@ -29659,7 +29681,9 @@
       <c r="H822" s="1">
         <v>31</v>
       </c>
-      <c r="I822" s="1"/>
+      <c r="I822" s="1">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="J822" s="1">
         <v>23.1</v>
       </c>
@@ -29692,7 +29716,9 @@
       <c r="H823" s="1">
         <v>1</v>
       </c>
-      <c r="I823" s="1"/>
+      <c r="I823" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J823" s="1">
         <v>26.9</v>
       </c>
@@ -29725,7 +29751,9 @@
       <c r="H824" s="1">
         <v>2</v>
       </c>
-      <c r="I824" s="1"/>
+      <c r="I824" s="1">
+        <v>0</v>
+      </c>
       <c r="J824" s="1">
         <v>24.8</v>
       </c>
@@ -29758,7 +29786,9 @@
       <c r="H825" s="1">
         <v>3</v>
       </c>
-      <c r="I825" s="1"/>
+      <c r="I825" s="1">
+        <v>4.8</v>
+      </c>
       <c r="J825" s="1">
         <v>23.9</v>
       </c>
@@ -29791,7 +29821,9 @@
       <c r="H826" s="1">
         <v>4</v>
       </c>
-      <c r="I826" s="1"/>
+      <c r="I826" s="1">
+        <v>11</v>
+      </c>
       <c r="J826" s="1">
         <v>25.3</v>
       </c>
@@ -29824,7 +29856,9 @@
       <c r="H827" s="1">
         <v>5</v>
       </c>
-      <c r="I827" s="1"/>
+      <c r="I827" s="1">
+        <v>0</v>
+      </c>
       <c r="J827" s="1">
         <v>26.5</v>
       </c>
@@ -29857,7 +29891,9 @@
       <c r="H828" s="1">
         <v>6</v>
       </c>
-      <c r="I828" s="1"/>
+      <c r="I828" s="1">
+        <v>0</v>
+      </c>
       <c r="J828" s="1">
         <v>23.7</v>
       </c>
@@ -29890,7 +29926,9 @@
       <c r="H829" s="1">
         <v>7</v>
       </c>
-      <c r="I829" s="1"/>
+      <c r="I829" s="1">
+        <v>8.6</v>
+      </c>
       <c r="J829" s="1">
         <v>24.8</v>
       </c>
@@ -29923,7 +29961,9 @@
       <c r="H830" s="1">
         <v>8</v>
       </c>
-      <c r="I830" s="1"/>
+      <c r="I830" s="1">
+        <v>0</v>
+      </c>
       <c r="J830" s="1">
         <v>27.5</v>
       </c>
@@ -29956,7 +29996,9 @@
       <c r="H831" s="1">
         <v>9</v>
       </c>
-      <c r="I831" s="1"/>
+      <c r="I831" s="1">
+        <v>0</v>
+      </c>
       <c r="J831" s="1">
         <v>26.2</v>
       </c>
@@ -29989,7 +30031,9 @@
       <c r="H832" s="1">
         <v>10</v>
       </c>
-      <c r="I832" s="1"/>
+      <c r="I832" s="1">
+        <v>0</v>
+      </c>
       <c r="J832" s="1">
         <v>21.1</v>
       </c>
@@ -30022,7 +30066,9 @@
       <c r="H833" s="1">
         <v>11</v>
       </c>
-      <c r="I833" s="1"/>
+      <c r="I833" s="1">
+        <v>3</v>
+      </c>
       <c r="J833" s="1">
         <v>27.4</v>
       </c>
@@ -30055,7 +30101,9 @@
       <c r="H834" s="1">
         <v>12</v>
       </c>
-      <c r="I834" s="1"/>
+      <c r="I834" s="1">
+        <v>3.3</v>
+      </c>
       <c r="J834" s="1">
         <v>27.3</v>
       </c>
@@ -30088,7 +30136,9 @@
       <c r="H835" s="1">
         <v>13</v>
       </c>
-      <c r="I835" s="1"/>
+      <c r="I835" s="1">
+        <v>9.1</v>
+      </c>
       <c r="J835" s="1">
         <v>23.1</v>
       </c>
@@ -30121,7 +30171,9 @@
       <c r="H836" s="1">
         <v>14</v>
       </c>
-      <c r="I836" s="1"/>
+      <c r="I836" s="1">
+        <v>23.8</v>
+      </c>
       <c r="J836" s="1">
         <v>22.2</v>
       </c>
@@ -30154,7 +30206,9 @@
       <c r="H837" s="1">
         <v>15</v>
       </c>
-      <c r="I837" s="1"/>
+      <c r="I837" s="1">
+        <v>9.6</v>
+      </c>
       <c r="J837" s="1">
         <v>26.9</v>
       </c>
@@ -30187,7 +30241,9 @@
       <c r="H838" s="1">
         <v>16</v>
       </c>
-      <c r="I838" s="1"/>
+      <c r="I838" s="1">
+        <v>16.399999999999999</v>
+      </c>
       <c r="J838" s="1">
         <v>27.4</v>
       </c>
@@ -30220,7 +30276,9 @@
       <c r="H839" s="1">
         <v>17</v>
       </c>
-      <c r="I839" s="1"/>
+      <c r="I839" s="1">
+        <v>9.4</v>
+      </c>
       <c r="J839" s="1">
         <v>26</v>
       </c>
@@ -30253,7 +30311,9 @@
       <c r="H840" s="1">
         <v>18</v>
       </c>
-      <c r="I840" s="1"/>
+      <c r="I840" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J840" s="1">
         <v>26.2</v>
       </c>
@@ -30286,7 +30346,9 @@
       <c r="H841" s="1">
         <v>19</v>
       </c>
-      <c r="I841" s="1"/>
+      <c r="I841" s="1">
+        <v>0</v>
+      </c>
       <c r="J841" s="1">
         <v>27.8</v>
       </c>
@@ -30319,7 +30381,9 @@
       <c r="H842" s="1">
         <v>20</v>
       </c>
-      <c r="I842" s="1"/>
+      <c r="I842" s="1">
+        <v>0</v>
+      </c>
       <c r="J842" s="1">
         <v>26.6</v>
       </c>
@@ -30352,7 +30416,9 @@
       <c r="H843" s="1">
         <v>21</v>
       </c>
-      <c r="I843" s="1"/>
+      <c r="I843" s="1">
+        <v>11</v>
+      </c>
       <c r="J843" s="1">
         <v>26.6</v>
       </c>
@@ -30385,7 +30451,9 @@
       <c r="H844" s="1">
         <v>22</v>
       </c>
-      <c r="I844" s="1"/>
+      <c r="I844" s="1">
+        <v>0.4</v>
+      </c>
       <c r="J844" s="1">
         <v>27.4</v>
       </c>
@@ -30418,7 +30486,9 @@
       <c r="H845" s="1">
         <v>23</v>
       </c>
-      <c r="I845" s="1"/>
+      <c r="I845" s="1">
+        <v>0</v>
+      </c>
       <c r="J845" s="1">
         <v>24.1</v>
       </c>
@@ -30451,7 +30521,9 @@
       <c r="H846" s="1">
         <v>24</v>
       </c>
-      <c r="I846" s="1"/>
+      <c r="I846" s="1">
+        <v>0</v>
+      </c>
       <c r="J846" s="1">
         <v>23.8</v>
       </c>
@@ -30484,7 +30556,9 @@
       <c r="H847" s="1">
         <v>25</v>
       </c>
-      <c r="I847" s="1"/>
+      <c r="I847" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J847" s="1">
         <v>24.9</v>
       </c>
@@ -30517,7 +30591,9 @@
       <c r="H848" s="1">
         <v>26</v>
       </c>
-      <c r="I848" s="1"/>
+      <c r="I848" s="1">
+        <v>24.4</v>
+      </c>
       <c r="J848" s="1">
         <v>24.6</v>
       </c>
@@ -30550,7 +30626,9 @@
       <c r="H849" s="1">
         <v>27</v>
       </c>
-      <c r="I849" s="1"/>
+      <c r="I849" s="1">
+        <v>0</v>
+      </c>
       <c r="J849" s="1">
         <v>26.4</v>
       </c>
@@ -30583,7 +30661,9 @@
       <c r="H850" s="1">
         <v>28</v>
       </c>
-      <c r="I850" s="1"/>
+      <c r="I850" s="1">
+        <v>4.5999999999999996</v>
+      </c>
       <c r="J850" s="1">
         <v>25.7</v>
       </c>
@@ -30616,7 +30696,9 @@
       <c r="H851" s="1">
         <v>29</v>
       </c>
-      <c r="I851" s="1"/>
+      <c r="I851" s="1">
+        <v>0</v>
+      </c>
       <c r="J851" s="1">
         <v>26.6</v>
       </c>
@@ -30649,7 +30731,9 @@
       <c r="H852" s="1">
         <v>30</v>
       </c>
-      <c r="I852" s="1"/>
+      <c r="I852" s="1">
+        <v>18.7</v>
+      </c>
       <c r="J852" s="1">
         <v>25.1</v>
       </c>
@@ -30682,7 +30766,9 @@
       <c r="H853" s="1">
         <v>1</v>
       </c>
-      <c r="I853" s="1"/>
+      <c r="I853" s="1">
+        <v>0</v>
+      </c>
       <c r="J853" s="1">
         <v>27.6</v>
       </c>
@@ -30715,7 +30801,9 @@
       <c r="H854" s="1">
         <v>2</v>
       </c>
-      <c r="I854" s="1"/>
+      <c r="I854" s="1">
+        <v>4.5999999999999996</v>
+      </c>
       <c r="J854" s="1">
         <v>25.3</v>
       </c>
@@ -30748,7 +30836,9 @@
       <c r="H855" s="1">
         <v>3</v>
       </c>
-      <c r="I855" s="1"/>
+      <c r="I855" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J855" s="1">
         <v>27.3</v>
       </c>
@@ -30781,7 +30871,9 @@
       <c r="H856" s="1">
         <v>4</v>
       </c>
-      <c r="I856" s="1"/>
+      <c r="I856" s="1">
+        <v>0</v>
+      </c>
       <c r="J856" s="1">
         <v>25.4</v>
       </c>
@@ -30814,7 +30906,9 @@
       <c r="H857" s="1">
         <v>5</v>
       </c>
-      <c r="I857" s="1"/>
+      <c r="I857" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J857" s="1">
         <v>27.2</v>
       </c>
@@ -30847,7 +30941,9 @@
       <c r="H858" s="1">
         <v>6</v>
       </c>
-      <c r="I858" s="1"/>
+      <c r="I858" s="1">
+        <v>0</v>
+      </c>
       <c r="J858" s="1">
         <v>26.9</v>
       </c>
@@ -30880,7 +30976,9 @@
       <c r="H859" s="1">
         <v>7</v>
       </c>
-      <c r="I859" s="1"/>
+      <c r="I859" s="1">
+        <v>0</v>
+      </c>
       <c r="J859" s="1">
         <v>28</v>
       </c>
@@ -30913,7 +31011,9 @@
       <c r="H860" s="1">
         <v>8</v>
       </c>
-      <c r="I860" s="1"/>
+      <c r="I860" s="1">
+        <v>16.8</v>
+      </c>
       <c r="J860" s="1">
         <v>24.6</v>
       </c>
@@ -30946,7 +31046,9 @@
       <c r="H861" s="1">
         <v>9</v>
       </c>
-      <c r="I861" s="1"/>
+      <c r="I861" s="1">
+        <v>11.7</v>
+      </c>
       <c r="J861" s="1">
         <v>24.8</v>
       </c>
@@ -30979,7 +31081,9 @@
       <c r="H862" s="1">
         <v>10</v>
       </c>
-      <c r="I862" s="1"/>
+      <c r="I862" s="1">
+        <v>0</v>
+      </c>
       <c r="J862" s="1">
         <v>24.3</v>
       </c>
@@ -31012,7 +31116,9 @@
       <c r="H863" s="1">
         <v>11</v>
       </c>
-      <c r="I863" s="1"/>
+      <c r="I863" s="1">
+        <v>0</v>
+      </c>
       <c r="J863" s="1">
         <v>27.5</v>
       </c>
@@ -31045,7 +31151,9 @@
       <c r="H864" s="1">
         <v>12</v>
       </c>
-      <c r="I864" s="1"/>
+      <c r="I864" s="1">
+        <v>0</v>
+      </c>
       <c r="J864" s="1">
         <v>28.7</v>
       </c>
@@ -31078,7 +31186,9 @@
       <c r="H865" s="1">
         <v>13</v>
       </c>
-      <c r="I865" s="1"/>
+      <c r="I865" s="1">
+        <v>0</v>
+      </c>
       <c r="J865" s="1">
         <v>27.1</v>
       </c>
@@ -31111,7 +31221,9 @@
       <c r="H866" s="1">
         <v>14</v>
       </c>
-      <c r="I866" s="1"/>
+      <c r="I866" s="1">
+        <v>0</v>
+      </c>
       <c r="J866" s="1">
         <v>26.9</v>
       </c>
@@ -31144,7 +31256,9 @@
       <c r="H867" s="1">
         <v>15</v>
       </c>
-      <c r="I867" s="1"/>
+      <c r="I867" s="1">
+        <v>0</v>
+      </c>
       <c r="J867" s="1">
         <v>26.9</v>
       </c>
@@ -31177,7 +31291,9 @@
       <c r="H868" s="1">
         <v>16</v>
       </c>
-      <c r="I868" s="1"/>
+      <c r="I868" s="1">
+        <v>0</v>
+      </c>
       <c r="J868" s="1">
         <v>28.2</v>
       </c>
@@ -31210,7 +31326,9 @@
       <c r="H869" s="1">
         <v>17</v>
       </c>
-      <c r="I869" s="1"/>
+      <c r="I869" s="1">
+        <v>0</v>
+      </c>
       <c r="J869" s="1">
         <v>28.2</v>
       </c>
@@ -31243,7 +31361,9 @@
       <c r="H870" s="1">
         <v>18</v>
       </c>
-      <c r="I870" s="1"/>
+      <c r="I870" s="1">
+        <v>0</v>
+      </c>
       <c r="J870" s="1">
         <v>28.5</v>
       </c>
@@ -31276,7 +31396,9 @@
       <c r="H871" s="1">
         <v>19</v>
       </c>
-      <c r="I871" s="1"/>
+      <c r="I871" s="1">
+        <v>0</v>
+      </c>
       <c r="J871" s="1">
         <v>28.6</v>
       </c>
@@ -31309,7 +31431,9 @@
       <c r="H872" s="1">
         <v>20</v>
       </c>
-      <c r="I872" s="1"/>
+      <c r="I872" s="1">
+        <v>0</v>
+      </c>
       <c r="J872" s="1">
         <v>26.9</v>
       </c>
@@ -31342,7 +31466,9 @@
       <c r="H873" s="1">
         <v>21</v>
       </c>
-      <c r="I873" s="1"/>
+      <c r="I873" s="1">
+        <v>0</v>
+      </c>
       <c r="J873" s="1">
         <v>27</v>
       </c>
@@ -31375,7 +31501,9 @@
       <c r="H874" s="1">
         <v>22</v>
       </c>
-      <c r="I874" s="1"/>
+      <c r="I874" s="1">
+        <v>0</v>
+      </c>
       <c r="J874" s="1">
         <v>26.7</v>
       </c>
@@ -31408,7 +31536,9 @@
       <c r="H875" s="1">
         <v>23</v>
       </c>
-      <c r="I875" s="1"/>
+      <c r="I875" s="1">
+        <v>1</v>
+      </c>
       <c r="J875" s="1">
         <v>26.3</v>
       </c>
@@ -31441,7 +31571,9 @@
       <c r="H876" s="1">
         <v>24</v>
       </c>
-      <c r="I876" s="1"/>
+      <c r="I876" s="1">
+        <v>0</v>
+      </c>
       <c r="J876" s="1">
         <v>27.6</v>
       </c>
@@ -31474,7 +31606,9 @@
       <c r="H877" s="1">
         <v>25</v>
       </c>
-      <c r="I877" s="1"/>
+      <c r="I877" s="1">
+        <v>0</v>
+      </c>
       <c r="J877" s="1">
         <v>27.6</v>
       </c>
@@ -31507,7 +31641,9 @@
       <c r="H878" s="1">
         <v>26</v>
       </c>
-      <c r="I878" s="1"/>
+      <c r="I878" s="1">
+        <v>0</v>
+      </c>
       <c r="J878" s="1">
         <v>27.6</v>
       </c>
@@ -31540,7 +31676,9 @@
       <c r="H879" s="1">
         <v>27</v>
       </c>
-      <c r="I879" s="1"/>
+      <c r="I879" s="1">
+        <v>0</v>
+      </c>
       <c r="J879" s="1">
         <v>28.2</v>
       </c>
@@ -31573,7 +31711,9 @@
       <c r="H880" s="1">
         <v>28</v>
       </c>
-      <c r="I880" s="1"/>
+      <c r="I880" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J880" s="1">
         <v>27</v>
       </c>
@@ -31606,7 +31746,9 @@
       <c r="H881" s="1">
         <v>29</v>
       </c>
-      <c r="I881" s="1"/>
+      <c r="I881" s="1">
+        <v>0</v>
+      </c>
       <c r="J881" s="1">
         <v>27.8</v>
       </c>
@@ -31639,7 +31781,9 @@
       <c r="H882" s="1">
         <v>30</v>
       </c>
-      <c r="I882" s="1"/>
+      <c r="I882" s="1">
+        <v>0</v>
+      </c>
       <c r="J882" s="1">
         <v>26.8</v>
       </c>
@@ -31672,7 +31816,9 @@
       <c r="H883" s="1">
         <v>31</v>
       </c>
-      <c r="I883" s="1"/>
+      <c r="I883" s="1">
+        <v>0</v>
+      </c>
       <c r="J883" s="1">
         <v>28.1</v>
       </c>
@@ -31705,7 +31851,9 @@
       <c r="H884" s="1">
         <v>1</v>
       </c>
-      <c r="I884" s="1"/>
+      <c r="I884" s="1">
+        <v>0</v>
+      </c>
       <c r="J884" s="1">
         <v>28.4</v>
       </c>
@@ -31738,7 +31886,9 @@
       <c r="H885" s="1">
         <v>2</v>
       </c>
-      <c r="I885" s="1"/>
+      <c r="I885" s="1">
+        <v>0</v>
+      </c>
       <c r="J885" s="1">
         <v>28.7</v>
       </c>
@@ -31771,7 +31921,9 @@
       <c r="H886" s="1">
         <v>3</v>
       </c>
-      <c r="I886" s="1"/>
+      <c r="I886" s="1">
+        <v>0</v>
+      </c>
       <c r="J886" s="1">
         <v>28.6</v>
       </c>
@@ -31804,7 +31956,9 @@
       <c r="H887" s="1">
         <v>4</v>
       </c>
-      <c r="I887" s="1"/>
+      <c r="I887" s="1">
+        <v>0</v>
+      </c>
       <c r="J887" s="1">
         <v>29</v>
       </c>
@@ -31837,7 +31991,9 @@
       <c r="H888" s="1">
         <v>5</v>
       </c>
-      <c r="I888" s="1"/>
+      <c r="I888" s="1">
+        <v>0</v>
+      </c>
       <c r="J888" s="1">
         <v>28.6</v>
       </c>
@@ -31870,7 +32026,9 @@
       <c r="H889" s="1">
         <v>6</v>
       </c>
-      <c r="I889" s="1"/>
+      <c r="I889" s="1">
+        <v>0</v>
+      </c>
       <c r="J889" s="1">
         <v>28.6</v>
       </c>
@@ -31903,7 +32061,9 @@
       <c r="H890" s="1">
         <v>7</v>
       </c>
-      <c r="I890" s="1"/>
+      <c r="I890" s="1">
+        <v>0</v>
+      </c>
       <c r="J890" s="1">
         <v>28</v>
       </c>
@@ -31936,7 +32096,9 @@
       <c r="H891" s="1">
         <v>8</v>
       </c>
-      <c r="I891" s="1"/>
+      <c r="I891" s="1">
+        <v>0</v>
+      </c>
       <c r="J891" s="1">
         <v>29</v>
       </c>
@@ -31969,7 +32131,9 @@
       <c r="H892" s="1">
         <v>9</v>
       </c>
-      <c r="I892" s="1"/>
+      <c r="I892" s="1">
+        <v>0</v>
+      </c>
       <c r="J892" s="1">
         <v>25.9</v>
       </c>
@@ -32002,7 +32166,9 @@
       <c r="H893" s="1">
         <v>10</v>
       </c>
-      <c r="I893" s="1"/>
+      <c r="I893" s="1">
+        <v>0</v>
+      </c>
       <c r="J893" s="1">
         <v>25.5</v>
       </c>
@@ -32035,7 +32201,9 @@
       <c r="H894" s="1">
         <v>11</v>
       </c>
-      <c r="I894" s="1"/>
+      <c r="I894" s="1">
+        <v>0</v>
+      </c>
       <c r="J894" s="1">
         <v>26.2</v>
       </c>
@@ -32068,7 +32236,9 @@
       <c r="H895" s="1">
         <v>12</v>
       </c>
-      <c r="I895" s="1"/>
+      <c r="I895" s="1">
+        <v>0</v>
+      </c>
       <c r="J895" s="1">
         <v>25.2</v>
       </c>
@@ -32101,7 +32271,9 @@
       <c r="H896" s="1">
         <v>13</v>
       </c>
-      <c r="I896" s="1"/>
+      <c r="I896" s="1">
+        <v>0</v>
+      </c>
       <c r="J896" s="1">
         <v>28</v>
       </c>
@@ -32134,7 +32306,9 @@
       <c r="H897" s="1">
         <v>14</v>
       </c>
-      <c r="I897" s="1"/>
+      <c r="I897" s="1">
+        <v>0</v>
+      </c>
       <c r="J897" s="1">
         <v>28</v>
       </c>
@@ -32167,7 +32341,9 @@
       <c r="H898" s="1">
         <v>15</v>
       </c>
-      <c r="I898" s="1"/>
+      <c r="I898" s="1">
+        <v>0</v>
+      </c>
       <c r="J898" s="1">
         <v>28.2</v>
       </c>
@@ -32200,7 +32376,9 @@
       <c r="H899" s="1">
         <v>16</v>
       </c>
-      <c r="I899" s="1"/>
+      <c r="I899" s="1">
+        <v>0</v>
+      </c>
       <c r="J899" s="1">
         <v>26.8</v>
       </c>
@@ -32233,7 +32411,9 @@
       <c r="H900" s="1">
         <v>17</v>
       </c>
-      <c r="I900" s="1"/>
+      <c r="I900" s="1">
+        <v>0</v>
+      </c>
       <c r="J900" s="1">
         <v>27.5</v>
       </c>
@@ -32266,7 +32446,9 @@
       <c r="H901" s="1">
         <v>18</v>
       </c>
-      <c r="I901" s="1"/>
+      <c r="I901" s="1">
+        <v>0</v>
+      </c>
       <c r="J901" s="1">
         <v>28.2</v>
       </c>
@@ -32299,7 +32481,9 @@
       <c r="H902" s="1">
         <v>19</v>
       </c>
-      <c r="I902" s="1"/>
+      <c r="I902" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J902" s="1">
         <v>28.5</v>
       </c>
@@ -32332,7 +32516,9 @@
       <c r="H903" s="1">
         <v>20</v>
       </c>
-      <c r="I903" s="1"/>
+      <c r="I903" s="1">
+        <v>0</v>
+      </c>
       <c r="J903" s="1">
         <v>27.9</v>
       </c>
@@ -32365,7 +32551,9 @@
       <c r="H904" s="1">
         <v>21</v>
       </c>
-      <c r="I904" s="1"/>
+      <c r="I904" s="1">
+        <v>0</v>
+      </c>
       <c r="J904" s="1">
         <v>26.4</v>
       </c>
@@ -32398,7 +32586,9 @@
       <c r="H905" s="1">
         <v>22</v>
       </c>
-      <c r="I905" s="1"/>
+      <c r="I905" s="1">
+        <v>0</v>
+      </c>
       <c r="J905" s="1">
         <v>25.4</v>
       </c>
@@ -32431,7 +32621,9 @@
       <c r="H906" s="1">
         <v>23</v>
       </c>
-      <c r="I906" s="1"/>
+      <c r="I906" s="1">
+        <v>0</v>
+      </c>
       <c r="J906" s="1">
         <v>27.2</v>
       </c>
@@ -32464,7 +32656,9 @@
       <c r="H907" s="1">
         <v>24</v>
       </c>
-      <c r="I907" s="1"/>
+      <c r="I907" s="1">
+        <v>0</v>
+      </c>
       <c r="J907" s="1">
         <v>26.9</v>
       </c>
@@ -32497,7 +32691,9 @@
       <c r="H908" s="1">
         <v>25</v>
       </c>
-      <c r="I908" s="1"/>
+      <c r="I908" s="1">
+        <v>0</v>
+      </c>
       <c r="J908" s="1">
         <v>26</v>
       </c>
@@ -32530,7 +32726,9 @@
       <c r="H909" s="1">
         <v>26</v>
       </c>
-      <c r="I909" s="1"/>
+      <c r="I909" s="1">
+        <v>0</v>
+      </c>
       <c r="J909" s="1">
         <v>26.1</v>
       </c>
@@ -32563,7 +32761,9 @@
       <c r="H910" s="1">
         <v>27</v>
       </c>
-      <c r="I910" s="1"/>
+      <c r="I910" s="1">
+        <v>0</v>
+      </c>
       <c r="J910" s="1">
         <v>26.5</v>
       </c>
@@ -32596,7 +32796,9 @@
       <c r="H911" s="1">
         <v>28</v>
       </c>
-      <c r="I911" s="1"/>
+      <c r="I911" s="1">
+        <v>0</v>
+      </c>
       <c r="J911" s="1">
         <v>27</v>
       </c>
@@ -32629,7 +32831,9 @@
       <c r="H912" s="1">
         <v>29</v>
       </c>
-      <c r="I912" s="1"/>
+      <c r="I912" s="1">
+        <v>0</v>
+      </c>
       <c r="J912" s="1">
         <v>27.6</v>
       </c>
@@ -32662,7 +32866,9 @@
       <c r="H913" s="1">
         <v>30</v>
       </c>
-      <c r="I913" s="1"/>
+      <c r="I913" s="1">
+        <v>0</v>
+      </c>
       <c r="J913" s="1">
         <v>27.7</v>
       </c>
@@ -32695,7 +32901,9 @@
       <c r="H914" s="1">
         <v>1</v>
       </c>
-      <c r="I914" s="1"/>
+      <c r="I914" s="1">
+        <v>0</v>
+      </c>
       <c r="J914" s="1">
         <v>27.7</v>
       </c>
@@ -32728,7 +32936,9 @@
       <c r="H915" s="1">
         <v>2</v>
       </c>
-      <c r="I915" s="1"/>
+      <c r="I915" s="1">
+        <v>0</v>
+      </c>
       <c r="J915" s="1">
         <v>28.5</v>
       </c>
@@ -32761,7 +32971,9 @@
       <c r="H916" s="1">
         <v>3</v>
       </c>
-      <c r="I916" s="1"/>
+      <c r="I916" s="1">
+        <v>0</v>
+      </c>
       <c r="J916" s="1">
         <v>28.1</v>
       </c>
@@ -32794,7 +33006,9 @@
       <c r="H917" s="1">
         <v>4</v>
       </c>
-      <c r="I917" s="1"/>
+      <c r="I917" s="1">
+        <v>0</v>
+      </c>
       <c r="J917" s="1">
         <v>29</v>
       </c>
@@ -32827,7 +33041,9 @@
       <c r="H918" s="1">
         <v>5</v>
       </c>
-      <c r="I918" s="1"/>
+      <c r="I918" s="1">
+        <v>0</v>
+      </c>
       <c r="J918" s="1">
         <v>29.2</v>
       </c>
@@ -32860,7 +33076,9 @@
       <c r="H919" s="1">
         <v>6</v>
       </c>
-      <c r="I919" s="1"/>
+      <c r="I919" s="1">
+        <v>0</v>
+      </c>
       <c r="J919" s="1">
         <v>28.4</v>
       </c>
@@ -32893,7 +33111,9 @@
       <c r="H920" s="1">
         <v>7</v>
       </c>
-      <c r="I920" s="1"/>
+      <c r="I920" s="1">
+        <v>0</v>
+      </c>
       <c r="J920" s="1">
         <v>27.6</v>
       </c>
@@ -32926,7 +33146,9 @@
       <c r="H921" s="1">
         <v>8</v>
       </c>
-      <c r="I921" s="1"/>
+      <c r="I921" s="1">
+        <v>0</v>
+      </c>
       <c r="J921" s="1">
         <v>27.1</v>
       </c>
@@ -32959,7 +33181,9 @@
       <c r="H922" s="1">
         <v>9</v>
       </c>
-      <c r="I922" s="1"/>
+      <c r="I922" s="1">
+        <v>0</v>
+      </c>
       <c r="J922" s="1">
         <v>27.1</v>
       </c>
@@ -32992,7 +33216,9 @@
       <c r="H923" s="1">
         <v>10</v>
       </c>
-      <c r="I923" s="1"/>
+      <c r="I923" s="1">
+        <v>0</v>
+      </c>
       <c r="J923" s="1">
         <v>27.4</v>
       </c>
@@ -33025,7 +33251,9 @@
       <c r="H924" s="1">
         <v>11</v>
       </c>
-      <c r="I924" s="1"/>
+      <c r="I924" s="1">
+        <v>0</v>
+      </c>
       <c r="J924" s="1">
         <v>27.7</v>
       </c>
@@ -33058,7 +33286,9 @@
       <c r="H925" s="1">
         <v>12</v>
       </c>
-      <c r="I925" s="1"/>
+      <c r="I925" s="1">
+        <v>0</v>
+      </c>
       <c r="J925" s="1">
         <v>27.7</v>
       </c>
@@ -33091,7 +33321,9 @@
       <c r="H926" s="1">
         <v>13</v>
       </c>
-      <c r="I926" s="1"/>
+      <c r="I926" s="1">
+        <v>0</v>
+      </c>
       <c r="J926" s="1">
         <v>28.6</v>
       </c>
@@ -33124,7 +33356,9 @@
       <c r="H927" s="1">
         <v>14</v>
       </c>
-      <c r="I927" s="1"/>
+      <c r="I927" s="1">
+        <v>0</v>
+      </c>
       <c r="J927" s="1">
         <v>29.1</v>
       </c>
@@ -33157,7 +33391,9 @@
       <c r="H928" s="1">
         <v>15</v>
       </c>
-      <c r="I928" s="1"/>
+      <c r="I928" s="1">
+        <v>0</v>
+      </c>
       <c r="J928" s="1">
         <v>29.4</v>
       </c>
@@ -33190,7 +33426,9 @@
       <c r="H929" s="1">
         <v>16</v>
       </c>
-      <c r="I929" s="1"/>
+      <c r="I929" s="1">
+        <v>0</v>
+      </c>
       <c r="J929" s="1">
         <v>28.8</v>
       </c>
@@ -33223,7 +33461,9 @@
       <c r="H930" s="1">
         <v>17</v>
       </c>
-      <c r="I930" s="1"/>
+      <c r="I930" s="1">
+        <v>0</v>
+      </c>
       <c r="J930" s="1">
         <v>28.8</v>
       </c>
@@ -33256,7 +33496,9 @@
       <c r="H931" s="1">
         <v>18</v>
       </c>
-      <c r="I931" s="1"/>
+      <c r="I931" s="1">
+        <v>0</v>
+      </c>
       <c r="J931" s="1">
         <v>28.6</v>
       </c>
@@ -33289,7 +33531,9 @@
       <c r="H932" s="1">
         <v>19</v>
       </c>
-      <c r="I932" s="1"/>
+      <c r="I932" s="1">
+        <v>0</v>
+      </c>
       <c r="J932" s="1">
         <v>25.8</v>
       </c>
@@ -33322,7 +33566,9 @@
       <c r="H933" s="1">
         <v>20</v>
       </c>
-      <c r="I933" s="1"/>
+      <c r="I933" s="1">
+        <v>0</v>
+      </c>
       <c r="J933" s="1">
         <v>29</v>
       </c>
@@ -33355,7 +33601,9 @@
       <c r="H934" s="1">
         <v>21</v>
       </c>
-      <c r="I934" s="1"/>
+      <c r="I934" s="1">
+        <v>0</v>
+      </c>
       <c r="J934" s="1">
         <v>29.5</v>
       </c>
@@ -33388,7 +33636,9 @@
       <c r="H935" s="1">
         <v>22</v>
       </c>
-      <c r="I935" s="1"/>
+      <c r="I935" s="1">
+        <v>0</v>
+      </c>
       <c r="J935" s="1">
         <v>25.5</v>
       </c>
@@ -33421,7 +33671,9 @@
       <c r="H936" s="1">
         <v>23</v>
       </c>
-      <c r="I936" s="1"/>
+      <c r="I936" s="1">
+        <v>0</v>
+      </c>
       <c r="J936" s="1">
         <v>27.7</v>
       </c>
@@ -33454,7 +33706,9 @@
       <c r="H937" s="1">
         <v>24</v>
       </c>
-      <c r="I937" s="1"/>
+      <c r="I937" s="1">
+        <v>0</v>
+      </c>
       <c r="J937" s="1">
         <v>29.4</v>
       </c>
@@ -33487,7 +33741,9 @@
       <c r="H938" s="1">
         <v>25</v>
       </c>
-      <c r="I938" s="1"/>
+      <c r="I938" s="1">
+        <v>0</v>
+      </c>
       <c r="J938" s="1">
         <v>29.7</v>
       </c>
@@ -33520,7 +33776,9 @@
       <c r="H939" s="1">
         <v>26</v>
       </c>
-      <c r="I939" s="1"/>
+      <c r="I939" s="1">
+        <v>0</v>
+      </c>
       <c r="J939" s="1">
         <v>29.9</v>
       </c>
@@ -33553,7 +33811,9 @@
       <c r="H940" s="1">
         <v>27</v>
       </c>
-      <c r="I940" s="1"/>
+      <c r="I940" s="1">
+        <v>0</v>
+      </c>
       <c r="J940" s="1">
         <v>29.4</v>
       </c>
@@ -33586,7 +33846,9 @@
       <c r="H941" s="1">
         <v>28</v>
       </c>
-      <c r="I941" s="1"/>
+      <c r="I941" s="1">
+        <v>0</v>
+      </c>
       <c r="J941" s="1">
         <v>29.4</v>
       </c>
@@ -33619,7 +33881,9 @@
       <c r="H942" s="1">
         <v>29</v>
       </c>
-      <c r="I942" s="1"/>
+      <c r="I942" s="1">
+        <v>0</v>
+      </c>
       <c r="J942" s="1">
         <v>29.3</v>
       </c>
@@ -33652,7 +33916,9 @@
       <c r="H943" s="1">
         <v>30</v>
       </c>
-      <c r="I943" s="1"/>
+      <c r="I943" s="1">
+        <v>0</v>
+      </c>
       <c r="J943" s="1">
         <v>28.2</v>
       </c>
@@ -33685,7 +33951,9 @@
       <c r="H944" s="1">
         <v>31</v>
       </c>
-      <c r="I944" s="1"/>
+      <c r="I944" s="1">
+        <v>0</v>
+      </c>
       <c r="J944" s="1">
         <v>28.3</v>
       </c>
@@ -33718,7 +33986,9 @@
       <c r="H945" s="1">
         <v>1</v>
       </c>
-      <c r="I945" s="1"/>
+      <c r="I945" s="1">
+        <v>0</v>
+      </c>
       <c r="J945" s="1">
         <v>25.2</v>
       </c>
@@ -33751,7 +34021,9 @@
       <c r="H946" s="1">
         <v>2</v>
       </c>
-      <c r="I946" s="1"/>
+      <c r="I946" s="1">
+        <v>0</v>
+      </c>
       <c r="J946" s="1">
         <v>27.3</v>
       </c>
@@ -33784,7 +34056,9 @@
       <c r="H947" s="1">
         <v>3</v>
       </c>
-      <c r="I947" s="1"/>
+      <c r="I947" s="1">
+        <v>0</v>
+      </c>
       <c r="J947" s="1">
         <v>28.5</v>
       </c>
@@ -33817,7 +34091,9 @@
       <c r="H948" s="1">
         <v>4</v>
       </c>
-      <c r="I948" s="1"/>
+      <c r="I948" s="1">
+        <v>0</v>
+      </c>
       <c r="J948" s="1">
         <v>29.8</v>
       </c>
@@ -33850,7 +34126,9 @@
       <c r="H949" s="1">
         <v>5</v>
       </c>
-      <c r="I949" s="1"/>
+      <c r="I949" s="1">
+        <v>0</v>
+      </c>
       <c r="J949" s="1">
         <v>28.8</v>
       </c>
@@ -33883,7 +34161,9 @@
       <c r="H950" s="1">
         <v>6</v>
       </c>
-      <c r="I950" s="1"/>
+      <c r="I950" s="1">
+        <v>0</v>
+      </c>
       <c r="J950" s="1">
         <v>29.7</v>
       </c>
@@ -33916,7 +34196,9 @@
       <c r="H951" s="1">
         <v>7</v>
       </c>
-      <c r="I951" s="1"/>
+      <c r="I951" s="1">
+        <v>0</v>
+      </c>
       <c r="J951" s="1">
         <v>29.6</v>
       </c>
@@ -33949,7 +34231,9 @@
       <c r="H952" s="1">
         <v>8</v>
       </c>
-      <c r="I952" s="1"/>
+      <c r="I952" s="1">
+        <v>0</v>
+      </c>
       <c r="J952" s="1">
         <v>30.6</v>
       </c>
@@ -33982,7 +34266,9 @@
       <c r="H953" s="1">
         <v>9</v>
       </c>
-      <c r="I953" s="1"/>
+      <c r="I953" s="1">
+        <v>0</v>
+      </c>
       <c r="J953" s="1">
         <v>29.2</v>
       </c>
@@ -34015,7 +34301,9 @@
       <c r="H954" s="1">
         <v>10</v>
       </c>
-      <c r="I954" s="1"/>
+      <c r="I954" s="1">
+        <v>0</v>
+      </c>
       <c r="J954" s="1">
         <v>26.9</v>
       </c>
@@ -34048,7 +34336,9 @@
       <c r="H955" s="1">
         <v>11</v>
       </c>
-      <c r="I955" s="1"/>
+      <c r="I955" s="1">
+        <v>0</v>
+      </c>
       <c r="J955" s="1">
         <v>30.6</v>
       </c>
@@ -34081,7 +34371,9 @@
       <c r="H956" s="1">
         <v>12</v>
       </c>
-      <c r="I956" s="1"/>
+      <c r="I956" s="1">
+        <v>0</v>
+      </c>
       <c r="J956" s="1">
         <v>30</v>
       </c>
@@ -34114,7 +34406,9 @@
       <c r="H957" s="1">
         <v>13</v>
       </c>
-      <c r="I957" s="1"/>
+      <c r="I957" s="1">
+        <v>0</v>
+      </c>
       <c r="J957" s="1">
         <v>29.3</v>
       </c>
@@ -34147,7 +34441,9 @@
       <c r="H958" s="1">
         <v>14</v>
       </c>
-      <c r="I958" s="1"/>
+      <c r="I958" s="1">
+        <v>0</v>
+      </c>
       <c r="J958" s="1">
         <v>29.6</v>
       </c>
@@ -34180,7 +34476,9 @@
       <c r="H959" s="1">
         <v>15</v>
       </c>
-      <c r="I959" s="1"/>
+      <c r="I959" s="1">
+        <v>0</v>
+      </c>
       <c r="J959" s="1">
         <v>28.7</v>
       </c>
@@ -34213,7 +34511,9 @@
       <c r="H960" s="1">
         <v>16</v>
       </c>
-      <c r="I960" s="1"/>
+      <c r="I960" s="1">
+        <v>0</v>
+      </c>
       <c r="J960" s="1">
         <v>25.6</v>
       </c>
@@ -34246,7 +34546,9 @@
       <c r="H961" s="1">
         <v>17</v>
       </c>
-      <c r="I961" s="1"/>
+      <c r="I961" s="1">
+        <v>0</v>
+      </c>
       <c r="J961" s="1">
         <v>27.4</v>
       </c>
@@ -34279,7 +34581,9 @@
       <c r="H962" s="1">
         <v>18</v>
       </c>
-      <c r="I962" s="1"/>
+      <c r="I962" s="1">
+        <v>0</v>
+      </c>
       <c r="J962" s="1">
         <v>27.3</v>
       </c>
@@ -34312,7 +34616,9 @@
       <c r="H963" s="1">
         <v>19</v>
       </c>
-      <c r="I963" s="1"/>
+      <c r="I963" s="1">
+        <v>0</v>
+      </c>
       <c r="J963" s="1">
         <v>28.5</v>
       </c>
@@ -34345,7 +34651,9 @@
       <c r="H964" s="1">
         <v>20</v>
       </c>
-      <c r="I964" s="1"/>
+      <c r="I964" s="1">
+        <v>0</v>
+      </c>
       <c r="J964" s="1">
         <v>28.2</v>
       </c>
@@ -34378,7 +34686,9 @@
       <c r="H965" s="1">
         <v>21</v>
       </c>
-      <c r="I965" s="1"/>
+      <c r="I965" s="1">
+        <v>0</v>
+      </c>
       <c r="J965" s="1">
         <v>25.9</v>
       </c>
@@ -34411,7 +34721,9 @@
       <c r="H966" s="1">
         <v>22</v>
       </c>
-      <c r="I966" s="1"/>
+      <c r="I966" s="1">
+        <v>0</v>
+      </c>
       <c r="J966" s="1">
         <v>24.4</v>
       </c>
@@ -34444,7 +34756,9 @@
       <c r="H967" s="1">
         <v>23</v>
       </c>
-      <c r="I967" s="1"/>
+      <c r="I967" s="1">
+        <v>0</v>
+      </c>
       <c r="J967" s="1">
         <v>27.8</v>
       </c>
@@ -34477,7 +34791,9 @@
       <c r="H968" s="1">
         <v>24</v>
       </c>
-      <c r="I968" s="1"/>
+      <c r="I968" s="1">
+        <v>0</v>
+      </c>
       <c r="J968" s="1">
         <v>27.2</v>
       </c>
@@ -34510,7 +34826,9 @@
       <c r="H969" s="1">
         <v>25</v>
       </c>
-      <c r="I969" s="1"/>
+      <c r="I969" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J969" s="1">
         <v>27.4</v>
       </c>
@@ -34543,7 +34861,9 @@
       <c r="H970" s="1">
         <v>26</v>
       </c>
-      <c r="I970" s="1"/>
+      <c r="I970" s="1">
+        <v>0</v>
+      </c>
       <c r="J970" s="1">
         <v>29.1</v>
       </c>
@@ -34576,7 +34896,9 @@
       <c r="H971" s="1">
         <v>27</v>
       </c>
-      <c r="I971" s="1"/>
+      <c r="I971" s="1">
+        <v>0</v>
+      </c>
       <c r="J971" s="1">
         <v>29.1</v>
       </c>
@@ -34609,7 +34931,9 @@
       <c r="H972" s="1">
         <v>28</v>
       </c>
-      <c r="I972" s="1"/>
+      <c r="I972" s="1">
+        <v>0</v>
+      </c>
       <c r="J972" s="1">
         <v>30.5</v>
       </c>
@@ -34642,7 +34966,9 @@
       <c r="H973" s="1">
         <v>29</v>
       </c>
-      <c r="I973" s="1"/>
+      <c r="I973" s="1">
+        <v>0</v>
+      </c>
       <c r="J973" s="1">
         <v>27.5</v>
       </c>
@@ -34675,7 +35001,9 @@
       <c r="H974" s="1">
         <v>30</v>
       </c>
-      <c r="I974" s="1"/>
+      <c r="I974" s="1">
+        <v>0</v>
+      </c>
       <c r="J974" s="1">
         <v>28</v>
       </c>
@@ -34708,7 +35036,9 @@
       <c r="H975" s="1">
         <v>31</v>
       </c>
-      <c r="I975" s="1"/>
+      <c r="I975" s="1">
+        <v>54.9</v>
+      </c>
       <c r="J975" s="1">
         <v>28.9</v>
       </c>
@@ -34741,7 +35071,9 @@
       <c r="H976" s="1">
         <v>1</v>
       </c>
-      <c r="I976" s="1"/>
+      <c r="I976" s="1">
+        <v>0</v>
+      </c>
       <c r="J976" s="1">
         <v>26.1</v>
       </c>
@@ -34774,7 +35106,9 @@
       <c r="H977" s="1">
         <v>2</v>
       </c>
-      <c r="I977" s="1"/>
+      <c r="I977" s="1">
+        <v>1.5</v>
+      </c>
       <c r="J977" s="1">
         <v>27.6</v>
       </c>
@@ -34807,7 +35141,9 @@
       <c r="H978" s="1">
         <v>3</v>
       </c>
-      <c r="I978" s="1"/>
+      <c r="I978" s="1">
+        <v>1</v>
+      </c>
       <c r="J978" s="1">
         <v>28.8</v>
       </c>
@@ -34840,7 +35176,9 @@
       <c r="H979" s="1">
         <v>4</v>
       </c>
-      <c r="I979" s="1"/>
+      <c r="I979" s="1">
+        <v>0.4</v>
+      </c>
       <c r="J979" s="1">
         <v>25.6</v>
       </c>
@@ -34873,7 +35211,9 @@
       <c r="H980" s="1">
         <v>5</v>
       </c>
-      <c r="I980" s="1"/>
+      <c r="I980" s="1">
+        <v>0</v>
+      </c>
       <c r="J980" s="1">
         <v>26.8</v>
       </c>
@@ -34906,7 +35246,9 @@
       <c r="H981" s="1">
         <v>6</v>
       </c>
-      <c r="I981" s="1"/>
+      <c r="I981" s="1">
+        <v>0</v>
+      </c>
       <c r="J981" s="1">
         <v>29.3</v>
       </c>
@@ -34939,7 +35281,9 @@
       <c r="H982" s="1">
         <v>7</v>
       </c>
-      <c r="I982" s="1"/>
+      <c r="I982" s="1">
+        <v>0.8</v>
+      </c>
       <c r="J982" s="1">
         <v>28.9</v>
       </c>
@@ -34972,7 +35316,9 @@
       <c r="H983" s="1">
         <v>8</v>
       </c>
-      <c r="I983" s="1"/>
+      <c r="I983" s="1">
+        <v>0</v>
+      </c>
       <c r="J983" s="1">
         <v>28</v>
       </c>
@@ -35005,7 +35351,9 @@
       <c r="H984" s="1">
         <v>9</v>
       </c>
-      <c r="I984" s="1"/>
+      <c r="I984" s="1">
+        <v>5.8</v>
+      </c>
       <c r="J984" s="1">
         <v>31.4</v>
       </c>
@@ -35038,7 +35386,9 @@
       <c r="H985" s="1">
         <v>10</v>
       </c>
-      <c r="I985" s="1"/>
+      <c r="I985" s="1">
+        <v>0</v>
+      </c>
       <c r="J985" s="1">
         <v>29.6</v>
       </c>
@@ -35071,7 +35421,9 @@
       <c r="H986" s="1">
         <v>11</v>
       </c>
-      <c r="I986" s="1"/>
+      <c r="I986" s="1">
+        <v>30.5</v>
+      </c>
       <c r="J986" s="1">
         <v>29.1</v>
       </c>
@@ -35104,7 +35456,9 @@
       <c r="H987" s="1">
         <v>12</v>
       </c>
-      <c r="I987" s="1"/>
+      <c r="I987" s="1">
+        <v>6.2</v>
+      </c>
       <c r="J987" s="1">
         <v>29.4</v>
       </c>
@@ -35137,7 +35491,9 @@
       <c r="H988" s="1">
         <v>13</v>
       </c>
-      <c r="I988" s="1"/>
+      <c r="I988" s="1">
+        <v>0</v>
+      </c>
       <c r="J988" s="1">
         <v>30.4</v>
       </c>
@@ -35170,7 +35526,9 @@
       <c r="H989" s="1">
         <v>14</v>
       </c>
-      <c r="I989" s="1"/>
+      <c r="I989" s="1">
+        <v>0</v>
+      </c>
       <c r="J989" s="1">
         <v>31</v>
       </c>
@@ -35203,7 +35561,9 @@
       <c r="H990" s="1">
         <v>15</v>
       </c>
-      <c r="I990" s="1"/>
+      <c r="I990" s="1">
+        <v>0</v>
+      </c>
       <c r="J990" s="1">
         <v>29.8</v>
       </c>
@@ -35236,7 +35596,9 @@
       <c r="H991" s="1">
         <v>16</v>
       </c>
-      <c r="I991" s="1"/>
+      <c r="I991" s="1">
+        <v>2.6</v>
+      </c>
       <c r="J991" s="1">
         <v>31.9</v>
       </c>
@@ -35269,7 +35631,9 @@
       <c r="H992" s="1">
         <v>17</v>
       </c>
-      <c r="I992" s="1"/>
+      <c r="I992" s="1">
+        <v>0.8</v>
+      </c>
       <c r="J992" s="1">
         <v>29</v>
       </c>
@@ -35302,7 +35666,9 @@
       <c r="H993" s="1">
         <v>18</v>
       </c>
-      <c r="I993" s="1"/>
+      <c r="I993" s="1">
+        <v>0</v>
+      </c>
       <c r="J993" s="1">
         <v>31</v>
       </c>
@@ -35335,7 +35701,9 @@
       <c r="H994" s="1">
         <v>19</v>
       </c>
-      <c r="I994" s="1"/>
+      <c r="I994" s="1">
+        <v>5.2</v>
+      </c>
       <c r="J994" s="1">
         <v>31.8</v>
       </c>
@@ -35368,7 +35736,9 @@
       <c r="H995" s="1">
         <v>20</v>
       </c>
-      <c r="I995" s="1"/>
+      <c r="I995" s="1">
+        <v>0</v>
+      </c>
       <c r="J995" s="1">
         <v>27.2</v>
       </c>
@@ -35401,7 +35771,9 @@
       <c r="H996" s="1">
         <v>21</v>
       </c>
-      <c r="I996" s="1"/>
+      <c r="I996" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J996" s="1">
         <v>27.5</v>
       </c>
@@ -35434,7 +35806,9 @@
       <c r="H997" s="1">
         <v>22</v>
       </c>
-      <c r="I997" s="1"/>
+      <c r="I997" s="1">
+        <v>0.4</v>
+      </c>
       <c r="J997" s="1">
         <v>27.5</v>
       </c>
@@ -35467,7 +35841,9 @@
       <c r="H998" s="1">
         <v>23</v>
       </c>
-      <c r="I998" s="1"/>
+      <c r="I998" s="1">
+        <v>0.4</v>
+      </c>
       <c r="J998" s="1">
         <v>28.4</v>
       </c>
@@ -35500,7 +35876,9 @@
       <c r="H999" s="1">
         <v>24</v>
       </c>
-      <c r="I999" s="1"/>
+      <c r="I999" s="1">
+        <v>0</v>
+      </c>
       <c r="J999" s="1">
         <v>28.3</v>
       </c>
@@ -35533,7 +35911,9 @@
       <c r="H1000" s="1">
         <v>25</v>
       </c>
-      <c r="I1000" s="1"/>
+      <c r="I1000" s="1">
+        <v>0</v>
+      </c>
       <c r="J1000" s="1">
         <v>29.5</v>
       </c>
@@ -35566,7 +35946,9 @@
       <c r="H1001" s="1">
         <v>26</v>
       </c>
-      <c r="I1001" s="1"/>
+      <c r="I1001" s="1">
+        <v>1.2</v>
+      </c>
       <c r="J1001" s="1">
         <v>31.6</v>
       </c>
@@ -35599,7 +35981,9 @@
       <c r="H1002" s="1">
         <v>27</v>
       </c>
-      <c r="I1002" s="1"/>
+      <c r="I1002" s="1">
+        <v>0</v>
+      </c>
       <c r="J1002" s="1">
         <v>32.1</v>
       </c>
@@ -35632,7 +36016,9 @@
       <c r="H1003" s="1">
         <v>28</v>
       </c>
-      <c r="I1003" s="1"/>
+      <c r="I1003" s="1">
+        <v>7.8</v>
+      </c>
       <c r="J1003" s="1">
         <v>31.5</v>
       </c>
@@ -35665,7 +36051,9 @@
       <c r="H1004" s="1">
         <v>29</v>
       </c>
-      <c r="I1004" s="1"/>
+      <c r="I1004" s="1">
+        <v>0</v>
+      </c>
       <c r="J1004" s="1">
         <v>30.1</v>
       </c>
@@ -35698,7 +36086,9 @@
       <c r="H1005" s="1">
         <v>30</v>
       </c>
-      <c r="I1005" s="1"/>
+      <c r="I1005" s="1">
+        <v>1.2</v>
+      </c>
       <c r="J1005" s="1">
         <v>24</v>
       </c>
@@ -35731,7 +36121,9 @@
       <c r="H1006" s="1">
         <v>1</v>
       </c>
-      <c r="I1006" s="1"/>
+      <c r="I1006" s="1">
+        <v>17.8</v>
+      </c>
       <c r="J1006" s="1">
         <v>28.3</v>
       </c>
@@ -35764,7 +36156,9 @@
       <c r="H1007" s="1">
         <v>2</v>
       </c>
-      <c r="I1007" s="1"/>
+      <c r="I1007" s="1">
+        <v>0</v>
+      </c>
       <c r="J1007" s="1">
         <v>27.1</v>
       </c>
@@ -35797,7 +36191,9 @@
       <c r="H1008" s="1">
         <v>3</v>
       </c>
-      <c r="I1008" s="1"/>
+      <c r="I1008" s="1">
+        <v>0</v>
+      </c>
       <c r="J1008" s="1">
         <v>25.9</v>
       </c>
@@ -35830,7 +36226,9 @@
       <c r="H1009" s="1">
         <v>4</v>
       </c>
-      <c r="I1009" s="1"/>
+      <c r="I1009" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J1009" s="1">
         <v>29.2</v>
       </c>
@@ -35863,7 +36261,9 @@
       <c r="H1010" s="1">
         <v>5</v>
       </c>
-      <c r="I1010" s="1"/>
+      <c r="I1010" s="1">
+        <v>0</v>
+      </c>
       <c r="J1010" s="1">
         <v>25.8</v>
       </c>
@@ -35896,7 +36296,9 @@
       <c r="H1011" s="1">
         <v>6</v>
       </c>
-      <c r="I1011" s="1"/>
+      <c r="I1011" s="1">
+        <v>0.4</v>
+      </c>
       <c r="J1011" s="1">
         <v>27.6</v>
       </c>
@@ -35929,7 +36331,9 @@
       <c r="H1012" s="1">
         <v>7</v>
       </c>
-      <c r="I1012" s="1"/>
+      <c r="I1012" s="1">
+        <v>0</v>
+      </c>
       <c r="J1012" s="1">
         <v>28.7</v>
       </c>
@@ -35962,7 +36366,9 @@
       <c r="H1013" s="1">
         <v>8</v>
       </c>
-      <c r="I1013" s="1"/>
+      <c r="I1013" s="1">
+        <v>3</v>
+      </c>
       <c r="J1013" s="1">
         <v>21.6</v>
       </c>
@@ -35995,7 +36401,9 @@
       <c r="H1014" s="1">
         <v>9</v>
       </c>
-      <c r="I1014" s="1"/>
+      <c r="I1014" s="1">
+        <v>9.8000000000000007</v>
+      </c>
       <c r="J1014" s="1">
         <v>23.4</v>
       </c>
@@ -36028,7 +36436,9 @@
       <c r="H1015" s="1">
         <v>10</v>
       </c>
-      <c r="I1015" s="1"/>
+      <c r="I1015" s="1">
+        <v>1</v>
+      </c>
       <c r="J1015" s="1">
         <v>25.8</v>
       </c>
@@ -36061,7 +36471,9 @@
       <c r="H1016" s="1">
         <v>11</v>
       </c>
-      <c r="I1016" s="1"/>
+      <c r="I1016" s="1">
+        <v>0</v>
+      </c>
       <c r="J1016" s="1">
         <v>20.6</v>
       </c>
@@ -36094,7 +36506,9 @@
       <c r="H1017" s="1">
         <v>12</v>
       </c>
-      <c r="I1017" s="1"/>
+      <c r="I1017" s="1">
+        <v>0</v>
+      </c>
       <c r="J1017" s="1">
         <v>23.6</v>
       </c>
@@ -36127,7 +36541,9 @@
       <c r="H1018" s="1">
         <v>13</v>
       </c>
-      <c r="I1018" s="1"/>
+      <c r="I1018" s="1">
+        <v>5.2</v>
+      </c>
       <c r="J1018" s="1">
         <v>28.2</v>
       </c>
@@ -36160,7 +36576,9 @@
       <c r="H1019" s="1">
         <v>14</v>
       </c>
-      <c r="I1019" s="1"/>
+      <c r="I1019" s="1">
+        <v>8.4</v>
+      </c>
       <c r="J1019" s="1">
         <v>28.9</v>
       </c>
@@ -36193,7 +36611,9 @@
       <c r="H1020" s="1">
         <v>15</v>
       </c>
-      <c r="I1020" s="1"/>
+      <c r="I1020" s="1">
+        <v>2</v>
+      </c>
       <c r="J1020" s="1">
         <v>29.9</v>
       </c>
@@ -36226,7 +36646,9 @@
       <c r="H1021" s="1">
         <v>16</v>
       </c>
-      <c r="I1021" s="1"/>
+      <c r="I1021" s="1">
+        <v>0</v>
+      </c>
       <c r="J1021" s="1">
         <v>28.3</v>
       </c>
@@ -36259,7 +36681,9 @@
       <c r="H1022" s="1">
         <v>17</v>
       </c>
-      <c r="I1022" s="1"/>
+      <c r="I1022" s="1">
+        <v>0.4</v>
+      </c>
       <c r="J1022" s="1">
         <v>28.2</v>
       </c>
@@ -36292,7 +36716,9 @@
       <c r="H1023" s="1">
         <v>18</v>
       </c>
-      <c r="I1023" s="1"/>
+      <c r="I1023" s="1">
+        <v>10.6</v>
+      </c>
       <c r="J1023" s="1">
         <v>24.7</v>
       </c>
@@ -36325,7 +36751,9 @@
       <c r="H1024" s="1">
         <v>19</v>
       </c>
-      <c r="I1024" s="1"/>
+      <c r="I1024" s="1">
+        <v>0</v>
+      </c>
       <c r="J1024" s="1">
         <v>28.4</v>
       </c>
@@ -36358,7 +36786,9 @@
       <c r="H1025" s="1">
         <v>20</v>
       </c>
-      <c r="I1025" s="1"/>
+      <c r="I1025" s="1">
+        <v>2</v>
+      </c>
       <c r="J1025" s="1">
         <v>26.4</v>
       </c>
@@ -36391,7 +36821,9 @@
       <c r="H1026" s="1">
         <v>21</v>
       </c>
-      <c r="I1026" s="1"/>
+      <c r="I1026" s="1">
+        <v>0</v>
+      </c>
       <c r="J1026" s="1">
         <v>25</v>
       </c>
@@ -36424,7 +36856,9 @@
       <c r="H1027" s="1">
         <v>22</v>
       </c>
-      <c r="I1027" s="1"/>
+      <c r="I1027" s="1">
+        <v>0</v>
+      </c>
       <c r="J1027" s="1">
         <v>27.3</v>
       </c>
@@ -36457,7 +36891,9 @@
       <c r="H1028" s="1">
         <v>23</v>
       </c>
-      <c r="I1028" s="1"/>
+      <c r="I1028" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J1028" s="1">
         <v>29.4</v>
       </c>
@@ -36490,7 +36926,9 @@
       <c r="H1029" s="1">
         <v>24</v>
       </c>
-      <c r="I1029" s="1"/>
+      <c r="I1029" s="1">
+        <v>4.2</v>
+      </c>
       <c r="J1029" s="1">
         <v>29.5</v>
       </c>
@@ -36523,7 +36961,9 @@
       <c r="H1030" s="1">
         <v>25</v>
       </c>
-      <c r="I1030" s="1"/>
+      <c r="I1030" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J1030" s="1">
         <v>30.5</v>
       </c>
@@ -36556,7 +36996,9 @@
       <c r="H1031" s="1">
         <v>26</v>
       </c>
-      <c r="I1031" s="1"/>
+      <c r="I1031" s="1">
+        <v>1.2</v>
+      </c>
       <c r="J1031" s="1">
         <v>29.4</v>
       </c>
@@ -36589,7 +37031,9 @@
       <c r="H1032" s="1">
         <v>27</v>
       </c>
-      <c r="I1032" s="1"/>
+      <c r="I1032" s="1">
+        <v>17.2</v>
+      </c>
       <c r="J1032" s="1">
         <v>28.9</v>
       </c>
@@ -36622,7 +37066,9 @@
       <c r="H1033" s="1">
         <v>28</v>
       </c>
-      <c r="I1033" s="1"/>
+      <c r="I1033" s="1">
+        <v>43.8</v>
+      </c>
       <c r="J1033" s="1">
         <v>29.4</v>
       </c>
@@ -36655,7 +37101,9 @@
       <c r="H1034" s="1">
         <v>29</v>
       </c>
-      <c r="I1034" s="1"/>
+      <c r="I1034" s="1">
+        <v>0</v>
+      </c>
       <c r="J1034" s="1">
         <v>28.5</v>
       </c>
@@ -36688,7 +37136,9 @@
       <c r="H1035" s="1">
         <v>30</v>
       </c>
-      <c r="I1035" s="1"/>
+      <c r="I1035" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J1035" s="1">
         <v>29.6</v>
       </c>
@@ -36721,7 +37171,9 @@
       <c r="H1036" s="1">
         <v>31</v>
       </c>
-      <c r="I1036" s="1"/>
+      <c r="I1036" s="1">
+        <v>14</v>
+      </c>
       <c r="J1036" s="1">
         <v>26.7</v>
       </c>
@@ -36754,7 +37206,9 @@
       <c r="H1037" s="1">
         <v>1</v>
       </c>
-      <c r="I1037" s="1"/>
+      <c r="I1037" s="1">
+        <v>22</v>
+      </c>
       <c r="J1037" s="1">
         <v>22.3</v>
       </c>
@@ -36787,7 +37241,9 @@
       <c r="H1038" s="1">
         <v>2</v>
       </c>
-      <c r="I1038" s="1"/>
+      <c r="I1038" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J1038" s="1">
         <v>25.1</v>
       </c>
@@ -36820,7 +37276,9 @@
       <c r="H1039" s="1">
         <v>3</v>
       </c>
-      <c r="I1039" s="1"/>
+      <c r="I1039" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J1039" s="1">
         <v>27.4</v>
       </c>
@@ -36853,7 +37311,9 @@
       <c r="H1040" s="1">
         <v>4</v>
       </c>
-      <c r="I1040" s="1"/>
+      <c r="I1040" s="1">
+        <v>5.4</v>
+      </c>
       <c r="J1040" s="1">
         <v>28.5</v>
       </c>
@@ -36886,7 +37346,9 @@
       <c r="H1041" s="1">
         <v>5</v>
       </c>
-      <c r="I1041" s="1"/>
+      <c r="I1041" s="1">
+        <v>0</v>
+      </c>
       <c r="J1041" s="1">
         <v>29</v>
       </c>
@@ -36919,7 +37381,9 @@
       <c r="H1042" s="1">
         <v>6</v>
       </c>
-      <c r="I1042" s="1"/>
+      <c r="I1042" s="1">
+        <v>0</v>
+      </c>
       <c r="J1042" s="1">
         <v>26</v>
       </c>
@@ -36952,7 +37416,9 @@
       <c r="H1043" s="1">
         <v>7</v>
       </c>
-      <c r="I1043" s="1"/>
+      <c r="I1043" s="1">
+        <v>1.8</v>
+      </c>
       <c r="J1043" s="1">
         <v>24.4</v>
       </c>
@@ -36985,7 +37451,9 @@
       <c r="H1044" s="1">
         <v>8</v>
       </c>
-      <c r="I1044" s="1"/>
+      <c r="I1044" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J1044" s="1">
         <v>24</v>
       </c>
@@ -37018,7 +37486,9 @@
       <c r="H1045" s="1">
         <v>9</v>
       </c>
-      <c r="I1045" s="1"/>
+      <c r="I1045" s="1">
+        <v>1.8</v>
+      </c>
       <c r="J1045" s="1">
         <v>28.3</v>
       </c>
@@ -37051,7 +37521,9 @@
       <c r="H1046" s="1">
         <v>10</v>
       </c>
-      <c r="I1046" s="1"/>
+      <c r="I1046" s="1">
+        <v>0.4</v>
+      </c>
       <c r="J1046" s="1">
         <v>24.8</v>
       </c>
@@ -37084,7 +37556,9 @@
       <c r="H1047" s="1">
         <v>11</v>
       </c>
-      <c r="I1047" s="1"/>
+      <c r="I1047" s="1">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="J1047" s="1">
         <v>25.7</v>
       </c>
@@ -37117,7 +37591,9 @@
       <c r="H1048" s="1">
         <v>12</v>
       </c>
-      <c r="I1048" s="1"/>
+      <c r="I1048" s="1">
+        <v>3</v>
+      </c>
       <c r="J1048" s="1">
         <v>25.2</v>
       </c>
@@ -37150,7 +37626,9 @@
       <c r="H1049" s="1">
         <v>13</v>
       </c>
-      <c r="I1049" s="1"/>
+      <c r="I1049" s="1">
+        <v>3</v>
+      </c>
       <c r="J1049" s="1">
         <v>27.6</v>
       </c>
@@ -37183,7 +37661,9 @@
       <c r="H1050" s="1">
         <v>14</v>
       </c>
-      <c r="I1050" s="1"/>
+      <c r="I1050" s="1">
+        <v>5</v>
+      </c>
       <c r="J1050" s="1">
         <v>22</v>
       </c>
@@ -37216,7 +37696,9 @@
       <c r="H1051" s="1">
         <v>15</v>
       </c>
-      <c r="I1051" s="1"/>
+      <c r="I1051" s="1">
+        <v>1.6</v>
+      </c>
       <c r="J1051" s="1">
         <v>26.8</v>
       </c>
@@ -37249,7 +37731,9 @@
       <c r="H1052" s="1">
         <v>16</v>
       </c>
-      <c r="I1052" s="1"/>
+      <c r="I1052" s="1">
+        <v>3.8</v>
+      </c>
       <c r="J1052" s="1">
         <v>22.6</v>
       </c>
@@ -37282,7 +37766,9 @@
       <c r="H1053" s="1">
         <v>17</v>
       </c>
-      <c r="I1053" s="1"/>
+      <c r="I1053" s="1">
+        <v>0</v>
+      </c>
       <c r="J1053" s="1">
         <v>24.5</v>
       </c>
@@ -37315,7 +37801,9 @@
       <c r="H1054" s="1">
         <v>18</v>
       </c>
-      <c r="I1054" s="1"/>
+      <c r="I1054" s="1">
+        <v>3.4</v>
+      </c>
       <c r="J1054" s="1">
         <v>24.6</v>
       </c>
@@ -37348,7 +37836,9 @@
       <c r="H1055" s="1">
         <v>19</v>
       </c>
-      <c r="I1055" s="1"/>
+      <c r="I1055" s="1">
+        <v>3.2</v>
+      </c>
       <c r="J1055" s="1">
         <v>27.3</v>
       </c>
@@ -37381,7 +37871,9 @@
       <c r="H1056" s="1">
         <v>20</v>
       </c>
-      <c r="I1056" s="1"/>
+      <c r="I1056" s="1">
+        <v>9.6</v>
+      </c>
       <c r="J1056" s="1">
         <v>28</v>
       </c>
@@ -37414,7 +37906,9 @@
       <c r="H1057" s="1">
         <v>21</v>
       </c>
-      <c r="I1057" s="1"/>
+      <c r="I1057" s="1">
+        <v>9.8000000000000007</v>
+      </c>
       <c r="J1057" s="1">
         <v>23.4</v>
       </c>
@@ -37447,7 +37941,9 @@
       <c r="H1058" s="1">
         <v>22</v>
       </c>
-      <c r="I1058" s="1"/>
+      <c r="I1058" s="1">
+        <v>0.4</v>
+      </c>
       <c r="J1058" s="1">
         <v>24.3</v>
       </c>
@@ -37480,7 +37976,9 @@
       <c r="H1059" s="1">
         <v>23</v>
       </c>
-      <c r="I1059" s="1"/>
+      <c r="I1059" s="1">
+        <v>7</v>
+      </c>
       <c r="J1059" s="1">
         <v>26.4</v>
       </c>
@@ -37513,7 +38011,9 @@
       <c r="H1060" s="1">
         <v>24</v>
       </c>
-      <c r="I1060" s="1"/>
+      <c r="I1060" s="1">
+        <v>11.5</v>
+      </c>
       <c r="J1060" s="1">
         <v>28.1</v>
       </c>
@@ -37546,7 +38046,9 @@
       <c r="H1061" s="1">
         <v>25</v>
       </c>
-      <c r="I1061" s="1"/>
+      <c r="I1061" s="1">
+        <v>10.8</v>
+      </c>
       <c r="J1061" s="1">
         <v>25.3</v>
       </c>
@@ -37579,7 +38081,9 @@
       <c r="H1062" s="1">
         <v>26</v>
       </c>
-      <c r="I1062" s="1"/>
+      <c r="I1062" s="1">
+        <v>10</v>
+      </c>
       <c r="J1062" s="1">
         <v>26</v>
       </c>
@@ -37612,7 +38116,9 @@
       <c r="H1063" s="1">
         <v>27</v>
       </c>
-      <c r="I1063" s="1"/>
+      <c r="I1063" s="1">
+        <v>0</v>
+      </c>
       <c r="J1063" s="1">
         <v>27.1</v>
       </c>
@@ -37645,7 +38151,9 @@
       <c r="H1064" s="1">
         <v>28</v>
       </c>
-      <c r="I1064" s="1"/>
+      <c r="I1064" s="1">
+        <v>0</v>
+      </c>
       <c r="J1064" s="1">
         <v>24.3</v>
       </c>
@@ -37678,7 +38186,9 @@
       <c r="H1065" s="1">
         <v>29</v>
       </c>
-      <c r="I1065" s="1"/>
+      <c r="I1065" s="1">
+        <v>7.2</v>
+      </c>
       <c r="J1065" s="1">
         <v>25.1</v>
       </c>
@@ -37711,7 +38221,9 @@
       <c r="H1066" s="1">
         <v>30</v>
       </c>
-      <c r="I1066" s="1"/>
+      <c r="I1066" s="1">
+        <v>0</v>
+      </c>
       <c r="J1066" s="1">
         <v>26.3</v>
       </c>
@@ -37744,7 +38256,9 @@
       <c r="H1067" s="1">
         <v>1</v>
       </c>
-      <c r="I1067" s="1"/>
+      <c r="I1067" s="1">
+        <v>0</v>
+      </c>
       <c r="J1067" s="1">
         <v>26</v>
       </c>
@@ -37777,7 +38291,9 @@
       <c r="H1068" s="1">
         <v>2</v>
       </c>
-      <c r="I1068" s="1"/>
+      <c r="I1068" s="1">
+        <v>1.7</v>
+      </c>
       <c r="J1068" s="1">
         <v>23.5</v>
       </c>
@@ -37810,7 +38326,9 @@
       <c r="H1069" s="1">
         <v>3</v>
       </c>
-      <c r="I1069" s="1"/>
+      <c r="I1069" s="1">
+        <v>0</v>
+      </c>
       <c r="J1069" s="1">
         <v>23.5</v>
       </c>
@@ -37843,7 +38361,9 @@
       <c r="H1070" s="1">
         <v>4</v>
       </c>
-      <c r="I1070" s="1"/>
+      <c r="I1070" s="1">
+        <v>0</v>
+      </c>
       <c r="J1070" s="1">
         <v>27.2</v>
       </c>
@@ -37876,7 +38396,9 @@
       <c r="H1071" s="1">
         <v>5</v>
       </c>
-      <c r="I1071" s="1"/>
+      <c r="I1071" s="1">
+        <v>2.9</v>
+      </c>
       <c r="J1071" s="1">
         <v>23.2</v>
       </c>
@@ -37909,7 +38431,9 @@
       <c r="H1072" s="1">
         <v>6</v>
       </c>
-      <c r="I1072" s="1"/>
+      <c r="I1072" s="1">
+        <v>1.2</v>
+      </c>
       <c r="J1072" s="1">
         <v>25.1</v>
       </c>
@@ -37942,7 +38466,9 @@
       <c r="H1073" s="1">
         <v>7</v>
       </c>
-      <c r="I1073" s="1"/>
+      <c r="I1073" s="1">
+        <v>13.3</v>
+      </c>
       <c r="J1073" s="1">
         <v>26.6</v>
       </c>
@@ -37975,7 +38501,9 @@
       <c r="H1074" s="1">
         <v>8</v>
       </c>
-      <c r="I1074" s="1"/>
+      <c r="I1074" s="1">
+        <v>0</v>
+      </c>
       <c r="J1074" s="1">
         <v>28.1</v>
       </c>
@@ -38008,7 +38536,9 @@
       <c r="H1075" s="1">
         <v>9</v>
       </c>
-      <c r="I1075" s="1"/>
+      <c r="I1075" s="1">
+        <v>1</v>
+      </c>
       <c r="J1075" s="1">
         <v>27</v>
       </c>
@@ -38041,7 +38571,9 @@
       <c r="H1076" s="1">
         <v>10</v>
       </c>
-      <c r="I1076" s="1"/>
+      <c r="I1076" s="1">
+        <v>0</v>
+      </c>
       <c r="J1076" s="1">
         <v>26.4</v>
       </c>
@@ -38074,7 +38606,9 @@
       <c r="H1077" s="1">
         <v>11</v>
       </c>
-      <c r="I1077" s="1"/>
+      <c r="I1077" s="1">
+        <v>0.3</v>
+      </c>
       <c r="J1077" s="1">
         <v>26.2</v>
       </c>
@@ -38107,7 +38641,9 @@
       <c r="H1078" s="1">
         <v>12</v>
       </c>
-      <c r="I1078" s="1"/>
+      <c r="I1078" s="1">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="J1078" s="1">
         <v>26.3</v>
       </c>
@@ -38140,7 +38676,9 @@
       <c r="H1079" s="1">
         <v>13</v>
       </c>
-      <c r="I1079" s="1"/>
+      <c r="I1079" s="1">
+        <v>0</v>
+      </c>
       <c r="J1079" s="1">
         <v>28</v>
       </c>
@@ -38173,7 +38711,9 @@
       <c r="H1080" s="1">
         <v>14</v>
       </c>
-      <c r="I1080" s="1"/>
+      <c r="I1080" s="1">
+        <v>0</v>
+      </c>
       <c r="J1080" s="1">
         <v>28.2</v>
       </c>
@@ -38206,7 +38746,9 @@
       <c r="H1081" s="1">
         <v>15</v>
       </c>
-      <c r="I1081" s="1"/>
+      <c r="I1081" s="1">
+        <v>2.4</v>
+      </c>
       <c r="J1081" s="1">
         <v>28.3</v>
       </c>
@@ -38239,7 +38781,9 @@
       <c r="H1082" s="1">
         <v>16</v>
       </c>
-      <c r="I1082" s="1"/>
+      <c r="I1082" s="1">
+        <v>0.3</v>
+      </c>
       <c r="J1082" s="1">
         <v>27.3</v>
       </c>
@@ -38272,7 +38816,9 @@
       <c r="H1083" s="1">
         <v>17</v>
       </c>
-      <c r="I1083" s="1"/>
+      <c r="I1083" s="1">
+        <v>0</v>
+      </c>
       <c r="J1083" s="1">
         <v>29.3</v>
       </c>
@@ -38305,7 +38851,9 @@
       <c r="H1084" s="1">
         <v>18</v>
       </c>
-      <c r="I1084" s="1"/>
+      <c r="I1084" s="1">
+        <v>0.1</v>
+      </c>
       <c r="J1084" s="1">
         <v>29.4</v>
       </c>
@@ -38338,7 +38886,9 @@
       <c r="H1085" s="1">
         <v>19</v>
       </c>
-      <c r="I1085" s="1"/>
+      <c r="I1085" s="1">
+        <v>0</v>
+      </c>
       <c r="J1085" s="1">
         <v>26.9</v>
       </c>
@@ -38371,7 +38921,9 @@
       <c r="H1086" s="1">
         <v>20</v>
       </c>
-      <c r="I1086" s="1"/>
+      <c r="I1086" s="1">
+        <v>0.2</v>
+      </c>
       <c r="J1086" s="1">
         <v>27.2</v>
       </c>
@@ -38404,7 +38956,9 @@
       <c r="H1087" s="1">
         <v>21</v>
       </c>
-      <c r="I1087" s="1"/>
+      <c r="I1087" s="1">
+        <v>8</v>
+      </c>
       <c r="J1087" s="1">
         <v>24.5</v>
       </c>
@@ -38437,7 +38991,9 @@
       <c r="H1088" s="1">
         <v>22</v>
       </c>
-      <c r="I1088" s="1"/>
+      <c r="I1088" s="1">
+        <v>0</v>
+      </c>
       <c r="J1088" s="1">
         <v>26.4</v>
       </c>
@@ -38470,7 +39026,9 @@
       <c r="H1089" s="1">
         <v>23</v>
       </c>
-      <c r="I1089" s="1"/>
+      <c r="I1089" s="1">
+        <v>0</v>
+      </c>
       <c r="J1089" s="1">
         <v>27.5</v>
       </c>
@@ -38503,7 +39061,9 @@
       <c r="H1090" s="1">
         <v>24</v>
       </c>
-      <c r="I1090" s="1"/>
+      <c r="I1090" s="1">
+        <v>0</v>
+      </c>
       <c r="J1090" s="1">
         <v>26.9</v>
       </c>
@@ -38536,7 +39096,9 @@
       <c r="H1091" s="1">
         <v>25</v>
       </c>
-      <c r="I1091" s="1"/>
+      <c r="I1091" s="1">
+        <v>2.6</v>
+      </c>
       <c r="J1091" s="1">
         <v>25.1</v>
       </c>
@@ -38569,7 +39131,9 @@
       <c r="H1092" s="1">
         <v>26</v>
       </c>
-      <c r="I1092" s="1"/>
+      <c r="I1092" s="1">
+        <v>21</v>
+      </c>
       <c r="J1092" s="1">
         <v>24.1</v>
       </c>
@@ -38602,7 +39166,9 @@
       <c r="H1093" s="1">
         <v>27</v>
       </c>
-      <c r="I1093" s="1"/>
+      <c r="I1093" s="1">
+        <v>0</v>
+      </c>
       <c r="J1093" s="1">
         <v>27.5</v>
       </c>
@@ -38635,7 +39201,9 @@
       <c r="H1094" s="1">
         <v>28</v>
       </c>
-      <c r="I1094" s="1"/>
+      <c r="I1094" s="1">
+        <v>0</v>
+      </c>
       <c r="J1094" s="1">
         <v>28.5</v>
       </c>
@@ -38668,7 +39236,9 @@
       <c r="H1095" s="1">
         <v>29</v>
       </c>
-      <c r="I1095" s="1"/>
+      <c r="I1095" s="1">
+        <v>41.6</v>
+      </c>
       <c r="J1095" s="1">
         <v>29</v>
       </c>
@@ -38701,7 +39271,9 @@
       <c r="H1096" s="1">
         <v>30</v>
       </c>
-      <c r="I1096" s="1"/>
+      <c r="I1096" s="1">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="J1096" s="1">
         <v>29.4</v>
       </c>
@@ -38734,7 +39306,9 @@
       <c r="H1097" s="1">
         <v>31</v>
       </c>
-      <c r="I1097" s="1"/>
+      <c r="I1097" s="1">
+        <v>4.3</v>
+      </c>
       <c r="J1097" s="1">
         <v>28.1</v>
       </c>

</xml_diff>